<commit_message>
updates to data hooks
</commit_message>
<xml_diff>
--- a/data/primary_studies/Eagle_et_al_2021/intermediate/Eagle_2021_material_and_methods.xlsx
+++ b/data/primary_studies/Eagle_et_al_2021/intermediate/Eagle_2021_material_and_methods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/CCRCN-Data-Library/data/primary_studies/Eagle_et_al_2021/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5BF29C-CE83-844F-969F-AADCA74939B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B845D508-548B-1443-9B6D-828D6E828091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39500" yWindow="500" windowWidth="24500" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5280" windowWidth="30920" windowHeight="10000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="material_and_methods" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
   <si>
     <t>coring_method</t>
   </si>
@@ -266,6 +266,33 @@
   </si>
   <si>
     <t>Eagle_et_al_2021</t>
+  </si>
+  <si>
+    <t>Plum</t>
+  </si>
+  <si>
+    <t>measured</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>russian corer</t>
+  </si>
+  <si>
+    <t>roots and rhizomes included</t>
+  </si>
+  <si>
+    <t>sediment not sieved</t>
+  </si>
+  <si>
+    <t>acid fumigation</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>organic carbon</t>
   </si>
 </sst>
 </file>
@@ -1121,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1400,31 +1427,59 @@
       <c r="B4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="H4" s="4">
+        <v>60</v>
+      </c>
+      <c r="I4" s="4">
+        <v>48</v>
+      </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
+      <c r="L4" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
+      <c r="R4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="S4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
+      <c r="X4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
+      <c r="AA4" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="AB4" s="4"/>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>

</xml_diff>

<commit_message>
work on furthering data hooks for Eagle and Okeefe-Suttle studies
</commit_message>
<xml_diff>
--- a/data/primary_studies/Eagle_et_al_2021/intermediate/Eagle_2021_material_and_methods.xlsx
+++ b/data/primary_studies/Eagle_et_al_2021/intermediate/Eagle_2021_material_and_methods.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/CCRCN-Data-Library/data/primary_studies/Eagle_et_al_2021/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B845D508-548B-1443-9B6D-828D6E828091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8565F6-97B2-7945-BE9A-D88601D08488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5280" windowWidth="30920" windowHeight="10000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27380" yWindow="2540" windowWidth="33220" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="material_and_methods" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="93">
   <si>
     <t>coring_method</t>
   </si>
@@ -293,6 +293,12 @@
   </si>
   <si>
     <t>organic carbon</t>
+  </si>
+  <si>
+    <t>each sample</t>
+  </si>
+  <si>
+    <t>core collection date</t>
   </si>
 </sst>
 </file>
@@ -1148,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1480,10 +1486,14 @@
       <c r="AA4" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AB4" s="4"/>
+      <c r="AB4" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
+      <c r="AE4" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="AF4" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
preparing Eagle data hook for manager's review
</commit_message>
<xml_diff>
--- a/data/primary_studies/Eagle_et_al_2021/intermediate/Eagle_2021_material_and_methods.xlsx
+++ b/data/primary_studies/Eagle_et_al_2021/intermediate/Eagle_2021_material_and_methods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/CCRCN-Data-Library/data/primary_studies/Eagle_et_al_2021/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8565F6-97B2-7945-BE9A-D88601D08488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08522C84-71FD-224F-B295-96935D5A97AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27380" yWindow="2540" windowWidth="33220" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="95">
   <si>
     <t>coring_method</t>
   </si>
@@ -268,9 +268,6 @@
     <t>Eagle_et_al_2021</t>
   </si>
   <si>
-    <t>Plum</t>
-  </si>
-  <si>
     <t>measured</t>
   </si>
   <si>
@@ -295,10 +292,19 @@
     <t>organic carbon</t>
   </si>
   <si>
-    <t>each sample</t>
-  </si>
-  <si>
     <t>core collection date</t>
+  </si>
+  <si>
+    <t>Plum software used</t>
+  </si>
+  <si>
+    <t>CRS</t>
+  </si>
+  <si>
+    <t>mass accumulation</t>
+  </si>
+  <si>
+    <t>selected intervals</t>
   </si>
 </sst>
 </file>
@@ -1434,13 +1440,13 @@
         <v>80</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1461,40 +1467,44 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="W4" s="4"/>
       <c r="X4" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z4" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="AA4" s="4" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="AB4" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
       <c r="AE4" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF4" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>